<commit_message>
Updated to be safe, after long time
</commit_message>
<xml_diff>
--- a/data/prayer_times.xlsx
+++ b/data/prayer_times.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="mBYpJY7GEBfC31WiX0qXqfIDpEJiceNbc71AYyjbwwg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="ObrLo4qXAN9SH4WmilGML52wilGVRwSJjheyn5TLBfs="/>
     </ext>
   </extLst>
 </workbook>
@@ -326,23 +326,23 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>0.17708333333333334</v>
+        <v>0.2638888888888889</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.5833333333333334</v>
+      <c r="B3" s="3">
+        <v>0.5625</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
-        <v>0.75</v>
+      <c r="B4" s="3">
+        <v>0.6979166666666666</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -350,7 +350,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>0.9097222222222222</v>
+        <v>0.8090277777777778</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
@@ -358,7 +358,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>0.9097222222222222</v>
+        <v>0.8645833333333334</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
keyEvent for closing added
</commit_message>
<xml_diff>
--- a/data/prayer_times.xlsx
+++ b/data/prayer_times.xlsx
@@ -326,7 +326,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>0.2638888888888889</v>
+        <v>0.2708333333333333</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
@@ -334,7 +334,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>0.5625</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
@@ -350,7 +350,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>0.8090277777777778</v>
+        <v>0.7951388888888888</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
@@ -358,7 +358,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>0.8645833333333334</v>
+        <v>0.8541666666666666</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Update Media and Prayer Times live from Files in App without App-Restart
</commit_message>
<xml_diff>
--- a/data/prayer_times.xlsx
+++ b/data/prayer_times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\LanguagePython\subhanTV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C0581B-5C37-449E-8590-80ADC42E83E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99497FF7-8B4D-441F-BBFE-4EE2CD665829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21936" yWindow="1380" windowWidth="12288" windowHeight="15276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10212" yWindow="1284" windowWidth="12288" windowHeight="15276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -323,7 +323,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>